<commit_message>
Put in and refined safeguards for checking the income statement. Went through and added try and except statements for a number of fields. The biggest problem that we will face is the different naming conventions when it comes to reporting numbers to the SEC. Need to figure out a better way to deal with the naming conventions other than massive try and except statements. However, if it does come to that then we'll need a way to remotely update the code to deal with the new names as they come along.
</commit_message>
<xml_diff>
--- a/WSIG DCF Template.xlsx
+++ b/WSIG DCF Template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17414"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crogstad\Dropbox\WSIG Stuff\Model Templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="E10E0BEBE4E57948235D8CBCCF6E22C0D8B71E58" xr6:coauthVersionLast="9" xr6:coauthVersionMax="9"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25275" windowHeight="12180" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25280" windowHeight="12180" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="1" r:id="rId1"/>
@@ -22,17 +16,22 @@
     <sheet name="Cash Flow Calculations" sheetId="10" r:id="rId7"/>
     <sheet name="DCF Output" sheetId="12" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>NT2</author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,12 +62,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>NT2</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="F12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="F14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="F15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="F16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="F17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="F24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="B26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -177,12 +176,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>NT2</author>
   </authors>
   <commentList>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="G3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="N3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -209,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="O3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="B30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -560,14 +559,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,7 +635,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -647,28 +646,28 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -676,9 +675,9 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -686,22 +685,22 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -716,10 +715,10 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -733,28 +732,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -769,39 +768,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -816,27 +815,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -848,17 +847,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -866,35 +865,35 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1168,7 +1167,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1220,7 +1219,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1445,15 +1444,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1518,21 +1517,25 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="13.7109375" customWidth="1"/>
+    <col min="2" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1543,7 +1546,7 @@
     <row r="2" spans="1:9">
       <c r="A2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>11</v>
       </c>
@@ -1781,7 +1784,7 @@
       <c r="G10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15" thickBot="1">
       <c r="A11" s="25" t="s">
         <v>21</v>
       </c>
@@ -1865,7 +1868,7 @@
       <c r="G17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+    <row r="19" spans="1:9" ht="15" thickBot="1">
       <c r="A19" s="25" t="s">
         <v>34</v>
       </c>
@@ -1959,7 +1962,7 @@
       </c>
       <c r="B26" s="86"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1">
+    <row r="28" spans="1:9" ht="15" thickBot="1">
       <c r="A28" s="25" t="s">
         <v>36</v>
       </c>
@@ -2053,7 +2056,7 @@
       </c>
       <c r="B35" s="86"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1">
+    <row r="37" spans="1:6" ht="15" thickBot="1">
       <c r="A37" s="25" t="s">
         <v>37</v>
       </c>
@@ -2151,25 +2154,30 @@
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -2201,7 +2209,7 @@
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1">
+    <row r="3" spans="1:17" ht="15" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>41</v>
       </c>
@@ -2586,7 +2594,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="47">
-        <f t="shared" ref="B12:D12" si="9">B9-B10+B11</f>
+        <f t="shared" ref="B12:F12" si="9">B9-B10</f>
         <v>0</v>
       </c>
       <c r="C12" s="47">
@@ -2598,15 +2606,15 @@
         <v>0</v>
       </c>
       <c r="E12" s="47">
-        <f>E9-E10+E11</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F12" s="47">
-        <f t="shared" ref="F12:G12" si="10">F9-F10+F11</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G12" s="47">
-        <f t="shared" si="10"/>
+        <f>G9-G10</f>
         <v>0</v>
       </c>
       <c r="H12" s="48"/>
@@ -2648,7 +2656,7 @@
       <c r="P13" s="46"/>
       <c r="Q13" s="21"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1">
+    <row r="14" spans="1:17" ht="15" thickBot="1">
       <c r="A14" s="25" t="s">
         <v>52</v>
       </c>
@@ -2657,43 +2665,43 @@
         <v>1896</v>
       </c>
       <c r="C14" s="40">
-        <f t="shared" ref="C14:L14" si="11">C3</f>
+        <f t="shared" ref="C14:L14" si="10">C3</f>
         <v>1897</v>
       </c>
       <c r="D14" s="40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1898</v>
       </c>
       <c r="E14" s="40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1899</v>
       </c>
       <c r="F14" s="40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1900</v>
       </c>
       <c r="G14" s="41" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>Current 1900</v>
       </c>
       <c r="H14" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1901F</v>
       </c>
       <c r="I14" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1902F</v>
       </c>
       <c r="J14" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1903F</v>
       </c>
       <c r="K14" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1904F</v>
       </c>
       <c r="L14" s="41" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1905F</v>
       </c>
       <c r="M14" s="43"/>
@@ -2785,7 +2793,7 @@
       </c>
       <c r="M16" s="46"/>
       <c r="N16" s="46">
-        <f t="shared" ref="N16" si="12">G16</f>
+        <f t="shared" ref="N16" si="11">G16</f>
         <v>0</v>
       </c>
       <c r="O16" s="87"/>
@@ -2814,7 +2822,7 @@
       <c r="P17" s="46"/>
       <c r="Q17" s="21"/>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1">
+    <row r="18" spans="1:17" ht="15" thickBot="1">
       <c r="A18" s="25" t="s">
         <v>55</v>
       </c>
@@ -2823,43 +2831,43 @@
         <v>1896</v>
       </c>
       <c r="C18" s="40">
-        <f t="shared" ref="C18:L18" si="13">C14</f>
+        <f t="shared" ref="C18:L18" si="12">C14</f>
         <v>1897</v>
       </c>
       <c r="D18" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1898</v>
       </c>
       <c r="E18" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1899</v>
       </c>
       <c r="F18" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1900</v>
       </c>
       <c r="G18" s="41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>Current 1900</v>
       </c>
       <c r="H18" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1901F</v>
       </c>
       <c r="I18" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1902F</v>
       </c>
       <c r="J18" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1903F</v>
       </c>
       <c r="K18" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1904F</v>
       </c>
       <c r="L18" s="41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1905F</v>
       </c>
       <c r="M18" s="43"/>
@@ -2896,7 +2904,7 @@
       </c>
       <c r="O19" s="87"/>
       <c r="P19" s="46">
-        <f t="shared" ref="P19:P30" si="14">IF($G$3="NA",F19,F19+N19-O19)</f>
+        <f t="shared" ref="P19:P30" si="13">IF($G$3="NA",F19,F19+N19-O19)</f>
         <v>0</v>
       </c>
       <c r="Q19" s="21"/>
@@ -2918,12 +2926,12 @@
       <c r="L20" s="20"/>
       <c r="M20" s="46"/>
       <c r="N20" s="46">
-        <f t="shared" ref="N20:N27" si="15">G20</f>
+        <f t="shared" ref="N20:N27" si="14">G20</f>
         <v>0</v>
       </c>
       <c r="O20" s="87"/>
       <c r="P20" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q20" s="21"/>
@@ -2945,12 +2953,12 @@
       <c r="L21" s="20"/>
       <c r="M21" s="46"/>
       <c r="N21" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O21" s="87"/>
       <c r="P21" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q21" s="21"/>
@@ -2972,12 +2980,12 @@
       <c r="L22" s="20"/>
       <c r="M22" s="46"/>
       <c r="N22" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O22" s="87"/>
       <c r="P22" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q22" s="21"/>
@@ -2999,12 +3007,12 @@
       <c r="L23" s="20"/>
       <c r="M23" s="46"/>
       <c r="N23" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O23" s="87"/>
       <c r="P23" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q23" s="21"/>
@@ -3026,12 +3034,12 @@
       <c r="L24" s="20"/>
       <c r="M24" s="46"/>
       <c r="N24" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O24" s="87"/>
       <c r="P24" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q24" s="21"/>
@@ -3053,12 +3061,12 @@
       <c r="L25" s="20"/>
       <c r="M25" s="46"/>
       <c r="N25" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O25" s="87"/>
       <c r="P25" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q25" s="21"/>
@@ -3080,12 +3088,12 @@
       <c r="L26" s="20"/>
       <c r="M26" s="46"/>
       <c r="N26" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O26" s="87"/>
       <c r="P26" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q26" s="21"/>
@@ -3107,12 +3115,12 @@
       <c r="L27" s="20"/>
       <c r="M27" s="46"/>
       <c r="N27" s="46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O27" s="87"/>
       <c r="P27" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q27" s="21"/>
@@ -3126,53 +3134,53 @@
         <v>0</v>
       </c>
       <c r="C28" s="46">
-        <f t="shared" ref="C28:F28" si="16">C22-C26-C27</f>
+        <f t="shared" ref="C28:F28" si="15">C22-C26-C27</f>
         <v>0</v>
       </c>
       <c r="D28" s="46">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="E28" s="46">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F28" s="46">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="G28" s="20">
-        <f t="shared" ref="G28" si="17">G22-G26-G27</f>
+        <f t="shared" ref="G28" si="16">G22-G26-G27</f>
         <v>0</v>
       </c>
       <c r="H28" s="46">
-        <f t="shared" ref="H28" si="18">H22-H26-H27</f>
+        <f t="shared" ref="H28" si="17">H22-H26-H27</f>
         <v>0</v>
       </c>
       <c r="I28" s="46">
-        <f t="shared" ref="I28" si="19">I22-I26-I27</f>
+        <f t="shared" ref="I28" si="18">I22-I26-I27</f>
         <v>0</v>
       </c>
       <c r="J28" s="46">
-        <f t="shared" ref="J28" si="20">J22-J26-J27</f>
+        <f t="shared" ref="J28" si="19">J22-J26-J27</f>
         <v>0</v>
       </c>
       <c r="K28" s="46">
-        <f t="shared" ref="K28" si="21">K22-K26-K27</f>
+        <f t="shared" ref="K28" si="20">K22-K26-K27</f>
         <v>0</v>
       </c>
       <c r="L28" s="20">
-        <f t="shared" ref="L28:N28" si="22">L22-L26-L27</f>
+        <f t="shared" ref="L28:N28" si="21">L22-L26-L27</f>
         <v>0</v>
       </c>
       <c r="M28" s="46"/>
       <c r="N28" s="46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="O28" s="21"/>
       <c r="P28" s="46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q28" s="21"/>
@@ -3186,23 +3194,23 @@
         <v>0</v>
       </c>
       <c r="C29" s="47">
-        <f t="shared" ref="C29:N29" si="23">C21-C24-C20+C23</f>
+        <f t="shared" ref="C29:N29" si="22">C21-C24-C20+C23</f>
         <v>0</v>
       </c>
       <c r="D29" s="47">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="E29" s="47">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="F29" s="47">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="G29" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H29" s="47">
@@ -3227,12 +3235,12 @@
       </c>
       <c r="M29" s="47"/>
       <c r="N29" s="47">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O29" s="47"/>
       <c r="P29" s="47">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q29" s="21"/>
@@ -3268,22 +3276,22 @@
         <v>0</v>
       </c>
       <c r="J30" s="49">
-        <f t="shared" ref="J30:L30" si="24">J29-I29</f>
+        <f t="shared" ref="J30:L30" si="23">J29-I29</f>
         <v>0</v>
       </c>
       <c r="K30" s="49">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L30" s="39">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="M30" s="50"/>
       <c r="N30" s="47"/>
       <c r="O30" s="50"/>
       <c r="P30" s="47">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q30" s="21"/>
@@ -3346,7 +3354,6 @@
       <c r="Q33" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="G4">
     <cfRule type="expression" dxfId="25" priority="10">
       <formula>$G$3="NA"</formula>
@@ -3388,25 +3395,29 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -3438,7 +3449,7 @@
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1">
+    <row r="3" spans="1:17" ht="15" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>41</v>
       </c>
@@ -4011,7 +4022,7 @@
       <c r="P13" s="53"/>
       <c r="Q13" s="21"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1">
+    <row r="14" spans="1:17" ht="15" thickBot="1">
       <c r="A14" s="25" t="s">
         <v>52</v>
       </c>
@@ -4219,7 +4230,7 @@
       <c r="P17" s="53"/>
       <c r="Q17" s="21"/>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1">
+    <row r="18" spans="1:17" ht="15" thickBot="1">
       <c r="A18" s="25" t="s">
         <v>55</v>
       </c>
@@ -4960,24 +4971,28 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -5009,7 +5024,7 @@
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1">
+    <row r="3" spans="1:17" ht="15" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>41</v>
       </c>
@@ -5582,7 +5597,7 @@
       <c r="P13" s="53"/>
       <c r="Q13" s="21"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1">
+    <row r="14" spans="1:17" ht="15" thickBot="1">
       <c r="A14" s="25" t="s">
         <v>52</v>
       </c>
@@ -5790,7 +5805,7 @@
       <c r="P17" s="53"/>
       <c r="Q17" s="21"/>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1">
+    <row r="18" spans="1:17" ht="15" thickBot="1">
       <c r="A18" s="25" t="s">
         <v>55</v>
       </c>
@@ -6531,20 +6546,24 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6691,23 +6710,28 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6716,7 +6740,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1">
+    <row r="3" spans="1:16" ht="15" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>80</v>
       </c>
@@ -6971,7 +6995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1">
+    <row r="8" spans="1:16" ht="15" thickBot="1">
       <c r="A8" s="34" t="s">
         <v>53</v>
       </c>
@@ -7129,7 +7153,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" thickBot="1">
+    <row r="12" spans="1:16" ht="15" thickBot="1">
       <c r="A12" s="25" t="s">
         <v>88</v>
       </c>
@@ -7388,7 +7412,7 @@
       </c>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1">
+    <row r="17" spans="1:16" ht="15" thickBot="1">
       <c r="A17" s="34" t="s">
         <v>53</v>
       </c>
@@ -7546,7 +7570,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" thickBot="1">
+    <row r="21" spans="1:16" ht="15" thickBot="1">
       <c r="A21" s="25" t="s">
         <v>89</v>
       </c>
@@ -7817,7 +7841,7 @@
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
     </row>
-    <row r="26" spans="1:16" ht="15.75" thickBot="1">
+    <row r="26" spans="1:16" ht="15" thickBot="1">
       <c r="A26" s="34" t="s">
         <v>53</v>
       </c>
@@ -7982,25 +8006,30 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -8008,7 +8037,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>91</v>
       </c>
@@ -8225,6 +8254,10 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>